<commit_message>
Fix typo on the source Excel file
</commit_message>
<xml_diff>
--- a/Analysis/KRM_Layer_Markers.xlsx
+++ b/Analysis/KRM_Layer_Markers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristenmaynard/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lcollado/Dropbox/Code/HumanPilot/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133CC101-36C7-1040-9CBE-6DBD0583EC60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32125B05-F6F3-8F4A-8B1F-7AFD024890B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24220" yWindow="3580" windowWidth="27640" windowHeight="20420" xr2:uid="{8BF5C150-72CC-9846-9AC1-D3E3EFD54F6D}"/>
+    <workbookView xWindow="19600" yWindow="2720" windowWidth="27640" windowHeight="20420" xr2:uid="{8BF5C150-72CC-9846-9AC1-D3E3EFD54F6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="89">
   <si>
     <t>Gene</t>
   </si>
@@ -655,8 +655,8 @@
   <dimension ref="A1:K82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2232,6 +2232,9 @@
       <c r="J45">
         <v>0</v>
       </c>
+      <c r="K45" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">

</xml_diff>